<commit_message>
birthday for default password and make validation for must change password not same with birthday
</commit_message>
<xml_diff>
--- a/public/dist/excel/template_import_user.xlsx
+++ b/public/dist/excel/template_import_user.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp8\htdocs\siballu\public\dist\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F35F4F4-416C-4337-A5DA-F8ABCA6B6384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1A6FA3-88F3-4F5E-A150-40AF51D72E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4B4C9E3E-0401-2A4D-BF0B-A9BDBED5A355}"/>
   </bookViews>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
-  <si>
-    <t>223942</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>P</t>
   </si>
@@ -78,6 +75,24 @@
   </si>
   <si>
     <t>number_id</t>
+  </si>
+  <si>
+    <t>birthday</t>
+  </si>
+  <si>
+    <t>2005-09-25</t>
+  </si>
+  <si>
+    <t>Jika kolom birthday diisi maka password menjadi 20050925</t>
+  </si>
+  <si>
+    <t>Jika kolom birthday kosong maka password menjadi random</t>
+  </si>
+  <si>
+    <t>22394222</t>
+  </si>
+  <si>
+    <t>22394213</t>
   </si>
 </sst>
 </file>
@@ -87,7 +102,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -103,6 +118,13 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -128,7 +150,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -145,6 +167,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA29094E-B216-8749-8BF4-90AEDF5AA86E}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -473,67 +497,81 @@
     <col min="5" max="5" width="32.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F3" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>2</v>
+      <c r="G3" s="6"/>
+      <c r="H3" s="7" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>